<commit_message>
agregué documentos al corpus
</commit_message>
<xml_diff>
--- a/Evaluacion/documents2.xlsx
+++ b/Evaluacion/documents2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t xml:space="preserve">P_IFT_160117_6_Acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_IFT_070218_83_AccUPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acta_43aOrd_011117_Acc</t>
   </si>
 </sst>
 </file>
@@ -179,13 +188,13 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9433198380567"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -312,7 +321,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Agregar documentos al corpus
</commit_message>
<xml_diff>
--- a/Evaluacion/documents2.xlsx
+++ b/Evaluacion/documents2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -30,52 +30,34 @@
     <t xml:space="preserve">Archivo</t>
   </si>
   <si>
+    <t xml:space="preserve">Año</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_IFT_161215_600_Acc</t>
+  </si>
+  <si>
     <t xml:space="preserve">P_IFT_090316_82_Acc</t>
   </si>
   <si>
-    <t xml:space="preserve">P_IFT_161215_600_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_170316_106_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_170316_118_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_200416_161_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_270416_196_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_160117_1_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nuevo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_160117_2_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_160117_3_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_160117_4_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_160117_5_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_160117_6_Acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P_IFT_070218_83_AccUPR</t>
+    <t xml:space="preserve">P_IFT_250117_27_Acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_IFT_310118_28_Acc.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_IFT_310118_30_AccUPR</t>
   </si>
   <si>
     <t xml:space="preserve">Victoria</t>
   </si>
   <si>
     <t xml:space="preserve">Acta_43aOrd_011117_Acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominio Ajeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_IFT_220217_94_Acc</t>
   </si>
 </sst>
 </file>
@@ -159,13 +141,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -185,17 +171,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2267206477733"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,54 +192,82 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,87 +275,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>